<commit_message>
Change EXP3 from 7x2 to 8x2 in BOM
</commit_message>
<xml_diff>
--- a/Source/Project Outputs for RUMBA_plus/V3D_RUMBA_plus_BOM_1_5_0.xlsx
+++ b/Source/Project Outputs for RUMBA_plus/V3D_RUMBA_plus_BOM_1_5_0.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Git\RUMBA-Plus\Source\Project Outputs for RUMBA_plus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA18DDD1-A93B-4B93-8FA6-DB5EB448FCD5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7904ACD8-2E06-451B-8B13-19551A60A775}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="9030" xr2:uid="{E2B0C553-4562-4409-BF40-3A64BE3F67AE}"/>
   </bookViews>
   <sheets>
     <sheet name="RUMBA_plus_BOM_1_3_2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="184">
   <si>
     <t>Designator</t>
   </si>
@@ -571,6 +571,12 @@
   </si>
   <si>
     <t>R40, R41, R42, R43, R54, R60, R61</t>
+  </si>
+  <si>
+    <t>Header, 8-Pin, Dual row</t>
+  </si>
+  <si>
+    <t>Header 8X2</t>
   </si>
 </sst>
 </file>
@@ -968,7 +974,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,10 +1370,10 @@
         <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>182</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>63</v>
+        <v>183</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>

</xml_diff>